<commit_message>
Added lots of admin files
</commit_message>
<xml_diff>
--- a/Admin Files/Gantt Chart.xlsx
+++ b/Admin Files/Gantt Chart.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Strung Along\strung-along\Admin Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4C6A929-ADBC-452B-A1FF-00BA6D390FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EF73A7-932A-4ACB-BA0B-EE0FC2AC10F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AA417BD-2748-4CDC-B273-67AFD46A09ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7AA417BD-2748-4CDC-B273-67AFD46A09ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semester 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semester 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,8 +35,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dylan Jarvis</author>
+  </authors>
+  <commentList>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{329C1839-31B4-4D3A-88AE-F8E9B38D4481}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dylan Jarvis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+PAX</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Timeline</t>
   </si>
@@ -140,13 +175,46 @@
   </si>
   <si>
     <t>Hello my name is Bill :)</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Movement Engine</t>
+  </si>
+  <si>
+    <t>Playable Game</t>
+  </si>
+  <si>
+    <t>Project Reporting</t>
+  </si>
+  <si>
+    <t>Finalise Player Controller</t>
+  </si>
+  <si>
+    <t>Finalise Level Manager</t>
+  </si>
+  <si>
+    <t>Bug Fixing</t>
+  </si>
+  <si>
+    <t>Act 3 Scenes (pending)</t>
+  </si>
+  <si>
+    <t>Finalise Models</t>
+  </si>
+  <si>
+    <t>Particle Effects</t>
+  </si>
+  <si>
+    <t>Socials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +236,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +272,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,25 +344,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -582,35 +699,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1A16FA-EB24-4514-B245-96CAEA5A6A81}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="8.88671875" style="12"/>
+    <col min="5" max="5" width="8.88671875" style="11"/>
     <col min="6" max="6" width="8.88671875" style="3"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -625,7 +742,7 @@
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -654,402 +771,404 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="O6" s="14"/>
-      <c r="Q6" s="14"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="O6" s="13"/>
+      <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="O7" s="14"/>
-      <c r="Q7" s="14"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="O7" s="13"/>
+      <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="O8" s="14"/>
-      <c r="Q8" s="14"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="O8" s="13"/>
+      <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="14"/>
-      <c r="R10" s="14"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="13"/>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="14"/>
-      <c r="R11" s="14"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+      <c r="R11" s="13"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="O13" s="14"/>
-      <c r="Q13" s="14"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="O13" s="13"/>
+      <c r="Q13" s="13"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="P15" s="14"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
       <c r="O17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1062,4 +1181,402 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132419D7-0B12-4B61-8A2F-521B918F2FFD}">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="8.88671875" style="11"/>
+    <col min="6" max="6" width="8.88671875" style="16"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="A15:M15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>